<commit_message>
dtype handling for test_id
</commit_message>
<xml_diff>
--- a/tests/Dummy Data.xlsx
+++ b/tests/Dummy Data.xlsx
@@ -86,6 +86,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -112,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -120,6 +123,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -399,8 +408,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
+      <c r="A2" s="2">
+        <v>1.1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -484,8 +493,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>1.0</v>
+      <c r="A2" s="3">
+        <v>1.1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -495,7 +504,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -506,7 +515,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -517,7 +526,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -528,8 +537,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1">
-        <v>1.0</v>
+      <c r="A6" s="3">
+        <v>1.1</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>20</v>
@@ -539,7 +548,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>2.0</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -550,7 +559,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1">
+      <c r="A8" s="4">
         <v>3.0</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -561,7 +570,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>4.0</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -572,8 +581,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1">
-        <v>1.0</v>
+      <c r="A10" s="3">
+        <v>1.1</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -583,7 +592,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1">
+      <c r="A11" s="4">
         <v>2.0</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -594,7 +603,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1">
+      <c r="A12" s="4">
         <v>3.0</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -605,7 +614,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>4.0</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -642,8 +651,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
+      <c r="A2" s="3">
+        <v>1.1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -675,8 +684,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1">
-        <v>1.0</v>
+      <c r="A5" s="3">
+        <v>1.1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>20</v>
@@ -730,8 +739,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1">
-        <v>1.0</v>
+      <c r="A10" s="3">
+        <v>1.1</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>

</xml_diff>